<commit_message>
Add data dictionary fulfillment function.
</commit_message>
<xml_diff>
--- a/DM/seed/Domain Data Template.xlsx
+++ b/DM/seed/Domain Data Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LiuZP\00 LiuZP\Code\Python\DM\seed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C27C54-A6C1-44C7-941A-B29751B755F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF521B6A-164E-48B4-9EF4-CA88AD656B8C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="618" activeTab="4" xr2:uid="{2106D2D4-3865-4892-A6F6-16BFFBD29CC0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="618" xr2:uid="{2106D2D4-3865-4892-A6F6-16BFFBD29CC0}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Activity" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Customer_Profile" sheetId="5" r:id="rId4"/>
     <sheet name="Location" sheetId="12" r:id="rId5"/>
     <sheet name="Checking_Query" sheetId="31" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="32" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="146">
   <si>
     <t>Customer_Address_Mailing</t>
   </si>
@@ -133,9 +132,6 @@
   </si>
   <si>
     <t>VA</t>
-  </si>
-  <si>
-    <t>VT</t>
   </si>
   <si>
     <t>Modeling</t>
@@ -474,6 +470,12 @@
   </si>
   <si>
     <t>dbo_D_LOCATION.FACILITY_HQ_NM</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>DE</t>
   </si>
 </sst>
 </file>
@@ -858,7 +860,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -973,11 +975,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -990,6 +989,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1317,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CBC1CF8-6993-481F-A8DB-AC849BEBAEE9}">
-  <dimension ref="A1:AI26"/>
+  <dimension ref="A1:AM26"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AH1" sqref="AH1:AI1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1328,199 +1333,219 @@
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="48" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="48" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="48" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="50" t="s">
+      <c r="S1" s="50"/>
+      <c r="T1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="51"/>
-      <c r="T1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="50" t="s">
+      <c r="W1" s="50"/>
+      <c r="X1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="50" t="s">
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="50" t="s">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="48" t="s">
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI1" s="51"/>
-    </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="47"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM1" s="50"/>
+    </row>
+    <row r="2" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="52"/>
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI2" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM2" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="16"/>
@@ -1552,22 +1577,26 @@
       <c r="AG3" s="16"/>
       <c r="AH3" s="39"/>
       <c r="AI3" s="36"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="36"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="11"/>
@@ -1599,22 +1628,26 @@
       <c r="AG4" s="11"/>
       <c r="AH4" s="40"/>
       <c r="AI4" s="37"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="23"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="40"/>
+      <c r="AM4" s="37"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="11"/>
@@ -1646,22 +1679,26 @@
       <c r="AG5" s="11"/>
       <c r="AH5" s="40"/>
       <c r="AI5" s="37"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="40"/>
+      <c r="AM5" s="37"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="11"/>
@@ -1693,16 +1730,20 @@
       <c r="AG6" s="11"/>
       <c r="AH6" s="40"/>
       <c r="AI6" s="37"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="40"/>
+      <c r="AM6" s="37"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="34"/>
       <c r="E7" s="34"/>
@@ -1736,16 +1777,20 @@
       <c r="AG7" s="11"/>
       <c r="AH7" s="40"/>
       <c r="AI7" s="37"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ7" s="23"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="40"/>
+      <c r="AM7" s="37"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -1779,16 +1824,20 @@
       <c r="AG8" s="11"/>
       <c r="AH8" s="40"/>
       <c r="AI8" s="37"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="40"/>
+      <c r="AM8" s="37"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -1822,16 +1871,20 @@
       <c r="AG9" s="11"/>
       <c r="AH9" s="40"/>
       <c r="AI9" s="37"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ9" s="23"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="40"/>
+      <c r="AM9" s="37"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
@@ -1865,16 +1918,20 @@
       <c r="AG10" s="11"/>
       <c r="AH10" s="40"/>
       <c r="AI10" s="37"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="40"/>
+      <c r="AM10" s="37"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
@@ -1908,22 +1965,26 @@
       <c r="AG11" s="11"/>
       <c r="AH11" s="40"/>
       <c r="AI11" s="37"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="40"/>
+      <c r="AM11" s="37"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="11"/>
@@ -1955,22 +2016,26 @@
       <c r="AG12" s="11"/>
       <c r="AH12" s="40"/>
       <c r="AI12" s="37"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="40"/>
+      <c r="AM12" s="37"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="11"/>
@@ -2002,22 +2067,26 @@
       <c r="AG13" s="11"/>
       <c r="AH13" s="40"/>
       <c r="AI13" s="37"/>
-    </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ13" s="23"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="40"/>
+      <c r="AM13" s="37"/>
+    </row>
+    <row r="14" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="11"/>
@@ -2049,22 +2118,26 @@
       <c r="AG14" s="11"/>
       <c r="AH14" s="40"/>
       <c r="AI14" s="37"/>
-    </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ14" s="23"/>
+      <c r="AK14" s="11"/>
+      <c r="AL14" s="40"/>
+      <c r="AM14" s="37"/>
+    </row>
+    <row r="15" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D15" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E15" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="11"/>
@@ -2096,16 +2169,20 @@
       <c r="AG15" s="11"/>
       <c r="AH15" s="40"/>
       <c r="AI15" s="37"/>
-    </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ15" s="23"/>
+      <c r="AK15" s="11"/>
+      <c r="AL15" s="40"/>
+      <c r="AM15" s="37"/>
+    </row>
+    <row r="16" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D16" s="34"/>
       <c r="E16" s="34"/>
@@ -2139,16 +2216,20 @@
       <c r="AG16" s="11"/>
       <c r="AH16" s="40"/>
       <c r="AI16" s="37"/>
-    </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ16" s="23"/>
+      <c r="AK16" s="11"/>
+      <c r="AL16" s="40"/>
+      <c r="AM16" s="37"/>
+    </row>
+    <row r="17" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A17" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D17" s="34"/>
       <c r="E17" s="34"/>
@@ -2182,16 +2263,20 @@
       <c r="AG17" s="11"/>
       <c r="AH17" s="40"/>
       <c r="AI17" s="37"/>
-    </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ17" s="23"/>
+      <c r="AK17" s="11"/>
+      <c r="AL17" s="40"/>
+      <c r="AM17" s="37"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D18" s="34"/>
       <c r="E18" s="34"/>
@@ -2225,22 +2310,26 @@
       <c r="AG18" s="11"/>
       <c r="AH18" s="40"/>
       <c r="AI18" s="37"/>
-    </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ18" s="23"/>
+      <c r="AK18" s="11"/>
+      <c r="AL18" s="40"/>
+      <c r="AM18" s="37"/>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D19" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E19" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="11"/>
@@ -2272,22 +2361,26 @@
       <c r="AG19" s="11"/>
       <c r="AH19" s="40"/>
       <c r="AI19" s="37"/>
-    </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ19" s="23"/>
+      <c r="AK19" s="11"/>
+      <c r="AL19" s="40"/>
+      <c r="AM19" s="37"/>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A20" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D20" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E20" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="11"/>
@@ -2319,22 +2412,26 @@
       <c r="AG20" s="11"/>
       <c r="AH20" s="40"/>
       <c r="AI20" s="37"/>
-    </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ20" s="23"/>
+      <c r="AK20" s="11"/>
+      <c r="AL20" s="40"/>
+      <c r="AM20" s="37"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A21" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="11"/>
@@ -2366,22 +2463,26 @@
       <c r="AG21" s="11"/>
       <c r="AH21" s="40"/>
       <c r="AI21" s="37"/>
-    </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ21" s="23"/>
+      <c r="AK21" s="11"/>
+      <c r="AL21" s="40"/>
+      <c r="AM21" s="37"/>
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A22" s="6" t="s">
         <v>19</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D22" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E22" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="11"/>
@@ -2413,22 +2514,26 @@
       <c r="AG22" s="11"/>
       <c r="AH22" s="40"/>
       <c r="AI22" s="37"/>
-    </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ22" s="23"/>
+      <c r="AK22" s="11"/>
+      <c r="AL22" s="40"/>
+      <c r="AM22" s="37"/>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A23" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B23" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D23" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E23" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="11"/>
@@ -2460,16 +2565,20 @@
       <c r="AG23" s="11"/>
       <c r="AH23" s="40"/>
       <c r="AI23" s="37"/>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ23" s="23"/>
+      <c r="AK23" s="11"/>
+      <c r="AL23" s="40"/>
+      <c r="AM23" s="37"/>
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A24" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D24" s="34"/>
       <c r="E24" s="34"/>
@@ -2503,22 +2612,26 @@
       <c r="AG24" s="11"/>
       <c r="AH24" s="40"/>
       <c r="AI24" s="37"/>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ24" s="23"/>
+      <c r="AK24" s="11"/>
+      <c r="AL24" s="40"/>
+      <c r="AM24" s="37"/>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A25" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C25" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E25" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="11"/>
@@ -2550,22 +2663,26 @@
       <c r="AG25" s="11"/>
       <c r="AH25" s="40"/>
       <c r="AI25" s="37"/>
-    </row>
-    <row r="26" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AJ25" s="23"/>
+      <c r="AK25" s="11"/>
+      <c r="AL25" s="40"/>
+      <c r="AM25" s="37"/>
+    </row>
+    <row r="26" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C26" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E26" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F26" s="21"/>
       <c r="G26" s="13"/>
@@ -2597,16 +2714,15 @@
       <c r="AG26" s="13"/>
       <c r="AH26" s="41"/>
       <c r="AI26" s="38"/>
+      <c r="AJ26" s="24"/>
+      <c r="AK26" s="13"/>
+      <c r="AL26" s="41"/>
+      <c r="AM26" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
+  <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
@@ -2618,17 +2734,25 @@
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7E46EEC-20EB-464F-AE3C-452FCBCE0E9B}">
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AM14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:Q1048576"/>
+    <sheetView topLeftCell="U1" workbookViewId="0">
+      <selection activeCell="AL1" sqref="AL1:AM1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2636,199 +2760,219 @@
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="48" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="48" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="48" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="50" t="s">
+      <c r="S1" s="50"/>
+      <c r="T1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="51"/>
-      <c r="T1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="50" t="s">
+      <c r="W1" s="50"/>
+      <c r="X1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="50" t="s">
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="50" t="s">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="48" t="s">
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI1" s="51"/>
-    </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="46"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM1" s="50"/>
+    </row>
+    <row r="2" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="51"/>
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI2" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM2" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="16"/>
@@ -2860,22 +3004,26 @@
       <c r="AG3" s="16"/>
       <c r="AH3" s="39"/>
       <c r="AI3" s="36"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="36"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="16"/>
@@ -2907,22 +3055,26 @@
       <c r="AG4" s="16"/>
       <c r="AH4" s="39"/>
       <c r="AI4" s="36"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="39"/>
+      <c r="AM4" s="36"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="11"/>
@@ -2954,22 +3106,26 @@
       <c r="AG5" s="11"/>
       <c r="AH5" s="40"/>
       <c r="AI5" s="37"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="40"/>
+      <c r="AM5" s="37"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="11"/>
@@ -3001,22 +3157,26 @@
       <c r="AG6" s="11"/>
       <c r="AH6" s="40"/>
       <c r="AI6" s="37"/>
-    </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="40"/>
+      <c r="AM6" s="37"/>
+    </row>
+    <row r="7" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="11"/>
@@ -3048,16 +3208,20 @@
       <c r="AG7" s="11"/>
       <c r="AH7" s="40"/>
       <c r="AI7" s="37"/>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ7" s="23"/>
+      <c r="AK7" s="11"/>
+      <c r="AL7" s="40"/>
+      <c r="AM7" s="37"/>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="34"/>
       <c r="E8" s="34"/>
@@ -3091,16 +3255,20 @@
       <c r="AG8" s="11"/>
       <c r="AH8" s="40"/>
       <c r="AI8" s="37"/>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ8" s="23"/>
+      <c r="AK8" s="11"/>
+      <c r="AL8" s="40"/>
+      <c r="AM8" s="37"/>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="34"/>
       <c r="E9" s="34"/>
@@ -3134,22 +3302,26 @@
       <c r="AG9" s="11"/>
       <c r="AH9" s="40"/>
       <c r="AI9" s="37"/>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ9" s="23"/>
+      <c r="AK9" s="11"/>
+      <c r="AL9" s="40"/>
+      <c r="AM9" s="37"/>
+    </row>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A10" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="11"/>
@@ -3181,22 +3353,26 @@
       <c r="AG10" s="11"/>
       <c r="AH10" s="40"/>
       <c r="AI10" s="37"/>
-    </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ10" s="23"/>
+      <c r="AK10" s="11"/>
+      <c r="AL10" s="40"/>
+      <c r="AM10" s="37"/>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A11" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="11"/>
@@ -3228,22 +3404,26 @@
       <c r="AG11" s="11"/>
       <c r="AH11" s="40"/>
       <c r="AI11" s="37"/>
-    </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ11" s="23"/>
+      <c r="AK11" s="11"/>
+      <c r="AL11" s="40"/>
+      <c r="AM11" s="37"/>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="11"/>
@@ -3275,22 +3455,26 @@
       <c r="AG12" s="11"/>
       <c r="AH12" s="40"/>
       <c r="AI12" s="37"/>
-    </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ12" s="23"/>
+      <c r="AK12" s="11"/>
+      <c r="AL12" s="40"/>
+      <c r="AM12" s="37"/>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="11"/>
@@ -3322,22 +3506,26 @@
       <c r="AG13" s="11"/>
       <c r="AH13" s="40"/>
       <c r="AI13" s="37"/>
-    </row>
-    <row r="14" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AJ13" s="23"/>
+      <c r="AK13" s="11"/>
+      <c r="AL13" s="40"/>
+      <c r="AM13" s="37"/>
+    </row>
+    <row r="14" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F14" s="21"/>
       <c r="G14" s="13"/>
@@ -3369,16 +3557,15 @@
       <c r="AG14" s="13"/>
       <c r="AH14" s="41"/>
       <c r="AI14" s="38"/>
+      <c r="AJ14" s="24"/>
+      <c r="AK14" s="13"/>
+      <c r="AL14" s="41"/>
+      <c r="AM14" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
+  <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -3390,6 +3577,13 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3397,10 +3591,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7549514-47DE-45EB-BE25-730292EFC949}">
-  <dimension ref="A1:AI7"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P1:Q1048576"/>
+    <sheetView topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AK12" sqref="AK12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3408,199 +3602,219 @@
     <col min="1" max="1" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A1" s="46" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.35">
+      <c r="A1" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="48" t="s">
+      <c r="B1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="49"/>
-      <c r="D1" s="50" t="s">
+      <c r="C1" s="48"/>
+      <c r="D1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="E1" s="51"/>
-      <c r="F1" s="48" t="s">
+      <c r="E1" s="50"/>
+      <c r="F1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="G1" s="49"/>
-      <c r="H1" s="50" t="s">
+      <c r="G1" s="48"/>
+      <c r="H1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="51"/>
-      <c r="J1" s="48" t="s">
+      <c r="I1" s="50"/>
+      <c r="J1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="49"/>
-      <c r="L1" s="50" t="s">
+      <c r="K1" s="48"/>
+      <c r="L1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="51"/>
-      <c r="N1" s="48" t="s">
+      <c r="M1" s="50"/>
+      <c r="N1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="49"/>
-      <c r="P1" s="48" t="s">
+      <c r="O1" s="48"/>
+      <c r="P1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="50" t="s">
+      <c r="S1" s="50"/>
+      <c r="T1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="U1" s="48"/>
+      <c r="V1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="S1" s="51"/>
-      <c r="T1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="U1" s="49"/>
-      <c r="V1" s="50" t="s">
+      <c r="W1" s="50"/>
+      <c r="X1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="W1" s="51"/>
-      <c r="X1" s="48" t="s">
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="50" t="s">
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="48" t="s">
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="50" t="s">
+      <c r="AE1" s="50"/>
+      <c r="AF1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="48" t="s">
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="AI1" s="51"/>
-    </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="47"/>
+      <c r="AI1" s="50"/>
+      <c r="AJ1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM1" s="50"/>
+    </row>
+    <row r="2" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="52"/>
       <c r="B2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="O2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="S2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="T2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="U2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="V2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Y2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Z2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AA2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AB2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AC2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AD2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AE2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AF2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AG2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AH2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AI2" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AK2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AM2" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A3" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="19"/>
       <c r="G3" s="16"/>
@@ -3632,22 +3846,26 @@
       <c r="AG3" s="16"/>
       <c r="AH3" s="39"/>
       <c r="AI3" s="36"/>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ3" s="22"/>
+      <c r="AK3" s="16"/>
+      <c r="AL3" s="39"/>
+      <c r="AM3" s="36"/>
+    </row>
+    <row r="4" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A4" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="19"/>
       <c r="G4" s="16"/>
@@ -3679,22 +3897,26 @@
       <c r="AG4" s="16"/>
       <c r="AH4" s="39"/>
       <c r="AI4" s="36"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="16"/>
+      <c r="AL4" s="39"/>
+      <c r="AM4" s="36"/>
+    </row>
+    <row r="5" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="11"/>
@@ -3726,22 +3948,26 @@
       <c r="AG5" s="11"/>
       <c r="AH5" s="40"/>
       <c r="AI5" s="37"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+      <c r="AJ5" s="23"/>
+      <c r="AK5" s="11"/>
+      <c r="AL5" s="40"/>
+      <c r="AM5" s="37"/>
+    </row>
+    <row r="6" spans="1:39" x14ac:dyDescent="0.35">
       <c r="A6" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="11"/>
@@ -3773,22 +3999,26 @@
       <c r="AG6" s="11"/>
       <c r="AH6" s="40"/>
       <c r="AI6" s="37"/>
-    </row>
-    <row r="7" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AJ6" s="23"/>
+      <c r="AK6" s="11"/>
+      <c r="AL6" s="40"/>
+      <c r="AM6" s="37"/>
+    </row>
+    <row r="7" spans="1:39" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="21"/>
       <c r="G7" s="13"/>
@@ -3820,16 +4050,15 @@
       <c r="AG7" s="13"/>
       <c r="AH7" s="41"/>
       <c r="AI7" s="38"/>
+      <c r="AJ7" s="24"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="41"/>
+      <c r="AM7" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
-    <mergeCell ref="AB1:AC1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
+  <mergeCells count="20">
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
     <mergeCell ref="T1:U1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:C1"/>
@@ -3841,6 +4070,13 @@
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="X1:Y1"/>
+    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="AB1:AC1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3848,10 +4084,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD8B9E0-6956-472F-8AED-5403C83B8FC7}">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AN14"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q1:R1048576"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AM1" sqref="AM1:AN1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3860,200 +4096,220 @@
     <col min="2" max="2" width="35.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="48" t="s">
+      <c r="F1" s="50"/>
+      <c r="G1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="48" t="s">
+      <c r="J1" s="50"/>
+      <c r="K1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="50" t="s">
+      <c r="L1" s="48"/>
+      <c r="M1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="48" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="49"/>
-      <c r="S1" s="50" t="s">
+      <c r="T1" s="50"/>
+      <c r="U1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" s="48"/>
+      <c r="W1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="49"/>
-      <c r="W1" s="50" t="s">
+      <c r="X1" s="50"/>
+      <c r="Y1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="50" t="s">
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="48" t="s">
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="50" t="s">
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="48" t="s">
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ1" s="51"/>
-    </row>
-    <row r="2" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="53"/>
-      <c r="B2" s="55"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN1" s="50"/>
+    </row>
+    <row r="2" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="54"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="P2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="R2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="T2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="V2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="X2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="Y2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AC2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AF2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AJ2" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="AK2" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL2" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM2" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN2" s="32" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="J2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="K2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="O2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="R2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="S2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="U2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="W2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="X2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="Y2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="AB2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="AC2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="AF2" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="AG2" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="AH2" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="AI2" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ2" s="32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+      <c r="B3" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>36</v>
-      </c>
       <c r="C3" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E3" s="42"/>
       <c r="F3" s="42"/>
@@ -4087,25 +4343,29 @@
       <c r="AH3" s="9"/>
       <c r="AI3" s="42"/>
       <c r="AJ3" s="43"/>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="43"/>
+    </row>
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F4" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="11"/>
@@ -4137,19 +4397,23 @@
       <c r="AH4" s="11"/>
       <c r="AI4" s="34"/>
       <c r="AJ4" s="37"/>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK4" s="20"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="37"/>
+    </row>
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="27" t="s">
-        <v>42</v>
-      </c>
       <c r="C5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="34"/>
@@ -4183,25 +4447,29 @@
       <c r="AH5" s="11"/>
       <c r="AI5" s="34"/>
       <c r="AJ5" s="37"/>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK5" s="20"/>
+      <c r="AL5" s="11"/>
+      <c r="AM5" s="34"/>
+      <c r="AN5" s="37"/>
+    </row>
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="27" t="s">
-        <v>44</v>
-      </c>
       <c r="C6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="11"/>
@@ -4233,25 +4501,29 @@
       <c r="AH6" s="11"/>
       <c r="AI6" s="34"/>
       <c r="AJ6" s="37"/>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="11"/>
+      <c r="AM6" s="34"/>
+      <c r="AN6" s="37"/>
+    </row>
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="27" t="s">
-        <v>46</v>
-      </c>
       <c r="C7" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="11"/>
@@ -4283,25 +4555,29 @@
       <c r="AH7" s="11"/>
       <c r="AI7" s="34"/>
       <c r="AJ7" s="37"/>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK7" s="20"/>
+      <c r="AL7" s="11"/>
+      <c r="AM7" s="34"/>
+      <c r="AN7" s="37"/>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E8" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F8" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G8" s="20"/>
       <c r="H8" s="11"/>
@@ -4333,25 +4609,29 @@
       <c r="AH8" s="11"/>
       <c r="AI8" s="34"/>
       <c r="AJ8" s="37"/>
-    </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK8" s="20"/>
+      <c r="AL8" s="11"/>
+      <c r="AM8" s="34"/>
+      <c r="AN8" s="37"/>
+    </row>
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E9" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G9" s="20"/>
       <c r="H9" s="11"/>
@@ -4383,25 +4663,29 @@
       <c r="AH9" s="11"/>
       <c r="AI9" s="34"/>
       <c r="AJ9" s="37"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="11"/>
+      <c r="AM9" s="34"/>
+      <c r="AN9" s="37"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G10" s="20"/>
       <c r="H10" s="11"/>
@@ -4433,25 +4717,29 @@
       <c r="AH10" s="11"/>
       <c r="AI10" s="34"/>
       <c r="AJ10" s="37"/>
-    </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="11"/>
+      <c r="AM10" s="34"/>
+      <c r="AN10" s="37"/>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C11" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F11" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="20"/>
       <c r="H11" s="11"/>
@@ -4483,25 +4771,29 @@
       <c r="AH11" s="11"/>
       <c r="AI11" s="34"/>
       <c r="AJ11" s="37"/>
-    </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK11" s="20"/>
+      <c r="AL11" s="11"/>
+      <c r="AM11" s="34"/>
+      <c r="AN11" s="37"/>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="27" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="27" t="s">
-        <v>56</v>
-      </c>
       <c r="C12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F12" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="11"/>
@@ -4533,25 +4825,29 @@
       <c r="AH12" s="11"/>
       <c r="AI12" s="34"/>
       <c r="AJ12" s="37"/>
-    </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="11"/>
+      <c r="AM12" s="34"/>
+      <c r="AN12" s="37"/>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>58</v>
-      </c>
       <c r="C13" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F13" s="34" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="11"/>
@@ -4583,25 +4879,29 @@
       <c r="AH13" s="11"/>
       <c r="AI13" s="34"/>
       <c r="AJ13" s="37"/>
-    </row>
-    <row r="14" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="11"/>
+      <c r="AM13" s="34"/>
+      <c r="AN13" s="37"/>
+    </row>
+    <row r="14" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B14" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>60</v>
-      </c>
       <c r="C14" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D14" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F14" s="35" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G14" s="21"/>
       <c r="H14" s="13"/>
@@ -4633,17 +4933,15 @@
       <c r="AH14" s="13"/>
       <c r="AI14" s="35"/>
       <c r="AJ14" s="38"/>
+      <c r="AK14" s="21"/>
+      <c r="AL14" s="13"/>
+      <c r="AM14" s="35"/>
+      <c r="AN14" s="38"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="AI1:AJ1"/>
-    <mergeCell ref="U1:V1"/>
-    <mergeCell ref="W1:X1"/>
-    <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="AA1:AB1"/>
-    <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AE1:AF1"/>
+  <mergeCells count="21">
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
     <mergeCell ref="S1:T1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="C1:D1"/>
@@ -4655,6 +4953,14 @@
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="AG1:AH1"/>
+    <mergeCell ref="AI1:AJ1"/>
+    <mergeCell ref="U1:V1"/>
+    <mergeCell ref="W1:X1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
+    <mergeCell ref="AC1:AD1"/>
+    <mergeCell ref="AE1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4662,10 +4968,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C0D7AB-943A-42F0-938E-A4DB31B9B282}">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AJ17" sqref="AJ17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4675,204 +4981,224 @@
     <col min="6" max="6" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
+      <c r="A1" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>38</v>
-      </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="49"/>
-      <c r="E1" s="50" t="s">
+      <c r="D1" s="48"/>
+      <c r="E1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="48" t="s">
+      <c r="F1" s="50"/>
+      <c r="G1" s="47" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="49"/>
-      <c r="I1" s="50" t="s">
+      <c r="H1" s="48"/>
+      <c r="I1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="51"/>
-      <c r="K1" s="48" t="s">
+      <c r="J1" s="50"/>
+      <c r="K1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="50" t="s">
+      <c r="L1" s="48"/>
+      <c r="M1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="51"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="48" t="s">
+      <c r="P1" s="48"/>
+      <c r="Q1" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="48"/>
+      <c r="S1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="R1" s="49"/>
-      <c r="S1" s="50" t="s">
+      <c r="T1" s="50"/>
+      <c r="U1" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="V1" s="48"/>
+      <c r="W1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="T1" s="51"/>
-      <c r="U1" s="48" t="s">
-        <v>78</v>
-      </c>
-      <c r="V1" s="49"/>
-      <c r="W1" s="50" t="s">
+      <c r="X1" s="50"/>
+      <c r="Y1" s="47" t="s">
         <v>71</v>
       </c>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="48" t="s">
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="50" t="s">
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="48" t="s">
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="50" t="s">
+      <c r="AF1" s="50"/>
+      <c r="AG1" s="47" t="s">
         <v>75</v>
       </c>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="48" t="s">
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="AJ1" s="51"/>
-    </row>
-    <row r="2" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="53"/>
-      <c r="B2" s="55"/>
+      <c r="AJ1" s="50"/>
+      <c r="AK1" s="47" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="49" t="s">
+        <v>145</v>
+      </c>
+      <c r="AN1" s="50"/>
+    </row>
+    <row r="2" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="54"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M2" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O2" s="17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P2" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S2" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="T2" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="U2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="W2" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="X2" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Y2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Z2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AA2" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AB2" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AC2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AD2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AE2" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AF2" s="45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AG2" s="29" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AH2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AI2" s="44" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="AJ2" s="45" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+        <v>33</v>
+      </c>
+      <c r="AK2" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL2" s="46" t="s">
+        <v>33</v>
+      </c>
+      <c r="AM2" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="AN2" s="45" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D3" s="9"/>
       <c r="E3" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F3" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G3" s="30"/>
       <c r="H3" s="9"/>
@@ -4904,19 +5230,23 @@
       <c r="AH3" s="9"/>
       <c r="AI3" s="42"/>
       <c r="AJ3" s="43"/>
-    </row>
-    <row r="4" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK3" s="30"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="42"/>
+      <c r="AN3" s="43"/>
+    </row>
+    <row r="4" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>82</v>
       </c>
       <c r="C4" s="8"/>
       <c r="D4" s="9"/>
       <c r="E4" s="42"/>
       <c r="F4" s="43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G4" s="30"/>
       <c r="H4" s="9"/>
@@ -4948,21 +5278,25 @@
       <c r="AH4" s="9"/>
       <c r="AI4" s="42"/>
       <c r="AJ4" s="43"/>
-    </row>
-    <row r="5" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="9"/>
+      <c r="AM4" s="42"/>
+      <c r="AN4" s="43"/>
+    </row>
+    <row r="5" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="42"/>
       <c r="F5" s="43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G5" s="30"/>
       <c r="H5" s="9"/>
@@ -4994,21 +5328,25 @@
       <c r="AH5" s="9"/>
       <c r="AI5" s="42"/>
       <c r="AJ5" s="43"/>
-    </row>
-    <row r="6" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK5" s="30"/>
+      <c r="AL5" s="9"/>
+      <c r="AM5" s="42"/>
+      <c r="AN5" s="43"/>
+    </row>
+    <row r="6" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="9"/>
       <c r="E6" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F6" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G6" s="30"/>
       <c r="H6" s="9"/>
@@ -5040,21 +5378,25 @@
       <c r="AH6" s="9"/>
       <c r="AI6" s="42"/>
       <c r="AJ6" s="43"/>
-    </row>
-    <row r="7" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK6" s="30"/>
+      <c r="AL6" s="9"/>
+      <c r="AM6" s="42"/>
+      <c r="AN6" s="43"/>
+    </row>
+    <row r="7" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="42"/>
       <c r="F7" s="43" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G7" s="30"/>
       <c r="H7" s="9"/>
@@ -5086,21 +5428,25 @@
       <c r="AH7" s="9"/>
       <c r="AI7" s="42"/>
       <c r="AJ7" s="43"/>
-    </row>
-    <row r="8" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK7" s="30"/>
+      <c r="AL7" s="9"/>
+      <c r="AM7" s="42"/>
+      <c r="AN7" s="43"/>
+    </row>
+    <row r="8" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="42"/>
       <c r="F8" s="43" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G8" s="30"/>
       <c r="H8" s="9"/>
@@ -5132,13 +5478,17 @@
       <c r="AH8" s="9"/>
       <c r="AI8" s="42"/>
       <c r="AJ8" s="43"/>
-    </row>
-    <row r="9" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="AK8" s="30"/>
+      <c r="AL8" s="9"/>
+      <c r="AM8" s="42"/>
+      <c r="AN8" s="43"/>
+    </row>
+    <row r="9" spans="1:40" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
@@ -5174,13 +5524,17 @@
       <c r="AH9" s="9"/>
       <c r="AI9" s="42"/>
       <c r="AJ9" s="43"/>
-    </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
+      <c r="AK9" s="30"/>
+      <c r="AL9" s="9"/>
+      <c r="AM9" s="42"/>
+      <c r="AN9" s="43"/>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="9"/>
@@ -5216,9 +5570,23 @@
       <c r="AH10" s="9"/>
       <c r="AI10" s="42"/>
       <c r="AJ10" s="43"/>
+      <c r="AK10" s="30"/>
+      <c r="AL10" s="9"/>
+      <c r="AM10" s="42"/>
+      <c r="AN10" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="AK1:AL1"/>
+    <mergeCell ref="AM1:AN1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
     <mergeCell ref="AI1:AJ1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -5230,14 +5598,6 @@
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AE1:AF1"/>
     <mergeCell ref="AG1:AH1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5260,453 +5620,453 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B15" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B18" t="s">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" t="s">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B25" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" t="s">
         <v>0</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B27" t="s">
         <v>1</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" t="s">
         <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C32" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
         <v>16</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B37" t="s">
         <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
         <v>91</v>
       </c>
-      <c r="B40" t="s">
-        <v>92</v>
-      </c>
       <c r="C40" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C41" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.35">
@@ -5714,10 +6074,10 @@
         <v>2</v>
       </c>
       <c r="B42" t="s">
+        <v>126</v>
+      </c>
+      <c r="C42" t="s">
         <v>127</v>
-      </c>
-      <c r="C42" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.35">
@@ -5725,10 +6085,10 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
+        <v>128</v>
+      </c>
+      <c r="C43" t="s">
         <v>129</v>
-      </c>
-      <c r="C43" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.35">
@@ -5736,10 +6096,10 @@
         <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C44" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.35">
@@ -5747,10 +6107,10 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.35">
@@ -5758,10 +6118,10 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.35">
@@ -5769,10 +6129,10 @@
         <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.35">
@@ -5780,10 +6140,10 @@
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -5791,10 +6151,10 @@
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -5802,10 +6162,10 @@
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C50" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -5813,10 +6173,10 @@
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C51" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -5824,10 +6184,10 @@
         <v>9</v>
       </c>
       <c r="B52" t="s">
+        <v>138</v>
+      </c>
+      <c r="C52" t="s">
         <v>139</v>
-      </c>
-      <c r="C52" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -5835,28 +6195,10 @@
         <v>9</v>
       </c>
       <c r="B53" t="s">
+        <v>140</v>
+      </c>
+      <c r="C53" t="s">
         <v>141</v>
-      </c>
-      <c r="C53" t="s">
-        <v>142</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBCE5DFB-EB52-48AD-9072-0AB5B4D73B13}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>